<commit_message>
added the csv database
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Android Dev\OutPatientProjec\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Git Projects\OutPatient\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20130" windowHeight="7590" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="plan" sheetId="1" r:id="rId1"/>
     <sheet name="Task" sheetId="2" r:id="rId2"/>
     <sheet name="Reminder" sheetId="3" r:id="rId3"/>
     <sheet name="Info" sheetId="4" r:id="rId4"/>
@@ -22,12 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="173">
   <si>
     <t>pid</t>
-  </si>
-  <si>
-    <t>pType</t>
   </si>
   <si>
     <t>name</t>
@@ -844,7 +841,7 @@
     <t>1418276837000</t>
   </si>
   <si>
-    <t>separater</t>
+    <t>plan_type</t>
   </si>
 </sst>
 </file>
@@ -1298,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1316,20 +1313,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>172</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>173</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -1339,7 +1334,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1350,7 +1345,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1361,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1372,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1383,7 +1378,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1394,7 +1389,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1443,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1461,87 +1456,84 @@
     <col min="9" max="16384" width="17.28515625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="19">
-        <v>1</v>
-      </c>
-      <c r="F2" s="15" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
-        <v>2</v>
-      </c>
-      <c r="B3" s="16">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="19">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="19">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
-        <v>3</v>
-      </c>
-      <c r="B4" s="16">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="19">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="19">
-        <v>2</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -1549,16 +1541,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="19">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="19">
-        <v>2</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -1566,14 +1558,14 @@
         <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="19">
         <v>3</v>
       </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -1581,16 +1573,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" s="19">
         <v>2</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -1598,16 +1590,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="18">
         <v>2</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -1615,16 +1607,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="18">
-        <v>2</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -1632,16 +1624,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="18">
         <v>1</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -1649,14 +1641,14 @@
         <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="19">
         <v>2</v>
       </c>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -1664,16 +1656,16 @@
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="19">
         <v>2</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -1681,16 +1673,16 @@
         <v>2</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="19">
         <v>3</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -1698,16 +1690,16 @@
         <v>2</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="18">
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -1715,16 +1707,16 @@
         <v>2</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="18">
         <v>2</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -1732,7 +1724,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="18">
         <v>2</v>
@@ -1746,13 +1738,13 @@
         <v>2</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="18">
         <v>3</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1763,13 +1755,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="18">
         <v>3</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1780,13 +1772,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="18">
         <v>1</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1797,7 +1789,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="18">
         <v>1</v>
@@ -1811,13 +1803,13 @@
         <v>3</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E21" s="18">
         <v>1</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1828,7 +1820,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22" s="18">
         <v>2</v>
@@ -1842,7 +1834,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E23" s="18">
         <v>2</v>
@@ -1856,7 +1848,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" s="18">
         <v>2</v>
@@ -1870,13 +1862,13 @@
         <v>3</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="18">
         <v>2</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1887,7 +1879,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26" s="18">
         <v>2</v>
@@ -1901,13 +1893,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" s="18">
         <v>2</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1918,13 +1910,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="18">
         <v>2</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1935,13 +1927,13 @@
         <v>3</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="18">
         <v>2</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1952,13 +1944,13 @@
         <v>3</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30" s="18">
         <v>2</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1969,7 +1961,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="18">
         <v>3</v>
@@ -1983,7 +1975,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E32" s="18">
         <v>3</v>
@@ -1997,7 +1989,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E33" s="18">
         <v>3</v>
@@ -2011,7 +2003,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="18">
         <v>3</v>
@@ -2025,7 +2017,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E35" s="18">
         <v>2</v>
@@ -2039,13 +2031,13 @@
         <v>4</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E36" s="18">
         <v>2</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2056,7 +2048,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E37" s="18">
         <v>3</v>
@@ -2070,7 +2062,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E38" s="18">
         <v>2</v>
@@ -2084,13 +2076,13 @@
         <v>4</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E39" s="18">
         <v>2</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2101,13 +2093,13 @@
         <v>4</v>
       </c>
       <c r="C40" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="18">
+        <v>2</v>
+      </c>
+      <c r="F40" s="22" t="s">
         <v>130</v>
-      </c>
-      <c r="E40" s="18">
-        <v>2</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2118,7 +2110,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2129,13 +2121,13 @@
         <v>5</v>
       </c>
       <c r="C42" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" s="18">
+        <v>2</v>
+      </c>
+      <c r="F42" s="18" t="s">
         <v>143</v>
-      </c>
-      <c r="E42" s="18">
-        <v>2</v>
-      </c>
-      <c r="F42" s="18" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2146,13 +2138,13 @@
         <v>5</v>
       </c>
       <c r="C43" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="18">
+        <v>2</v>
+      </c>
+      <c r="F43" s="18" t="s">
         <v>145</v>
-      </c>
-      <c r="E43" s="18">
-        <v>2</v>
-      </c>
-      <c r="F43" s="18" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2163,13 +2155,13 @@
         <v>5</v>
       </c>
       <c r="C44" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" s="18">
+        <v>2</v>
+      </c>
+      <c r="F44" s="18" t="s">
         <v>147</v>
-      </c>
-      <c r="E44" s="18">
-        <v>2</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2180,13 +2172,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="18">
+        <v>2</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="E45" s="18">
-        <v>2</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2197,7 +2189,7 @@
         <v>5</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E46" s="18">
         <v>2</v>
@@ -2211,13 +2203,13 @@
         <v>5</v>
       </c>
       <c r="C47" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="18">
+        <v>2</v>
+      </c>
+      <c r="F47" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="E47" s="18">
-        <v>2</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2228,7 +2220,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" s="18">
         <v>2</v>
@@ -2242,7 +2234,7 @@
         <v>5</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E49" s="18">
         <v>2</v>
@@ -2256,13 +2248,13 @@
         <v>5</v>
       </c>
       <c r="C50" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E50" s="18">
+        <v>2</v>
+      </c>
+      <c r="F50" s="18" t="s">
         <v>156</v>
-      </c>
-      <c r="E50" s="18">
-        <v>2</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2273,13 +2265,13 @@
         <v>5</v>
       </c>
       <c r="C51" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E51" s="18">
+        <v>2</v>
+      </c>
+      <c r="F51" s="18" t="s">
         <v>158</v>
-      </c>
-      <c r="E51" s="18">
-        <v>2</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2290,7 +2282,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="18">
         <v>2</v>
@@ -2304,13 +2296,13 @@
         <v>6</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E53" s="18">
         <v>1</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2321,13 +2313,13 @@
         <v>6</v>
       </c>
       <c r="C54" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="18">
+        <v>2</v>
+      </c>
+      <c r="F54" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="E54" s="18">
-        <v>2</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2338,13 +2330,13 @@
         <v>6</v>
       </c>
       <c r="C55" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="18">
+        <v>2</v>
+      </c>
+      <c r="F55" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="E55" s="18">
-        <v>2</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2355,13 +2347,13 @@
         <v>6</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="18">
+        <v>1</v>
+      </c>
+      <c r="F56" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="E56" s="18">
-        <v>1</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2372,13 +2364,13 @@
         <v>6</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E57" s="18">
         <v>2</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2389,13 +2381,13 @@
         <v>6</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E58" s="18">
         <v>2</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2406,13 +2398,13 @@
         <v>6</v>
       </c>
       <c r="C59" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E59" s="18">
+        <v>2</v>
+      </c>
+      <c r="F59" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="E59" s="18">
-        <v>2</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2423,13 +2415,13 @@
         <v>6</v>
       </c>
       <c r="C60" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="E60" s="18">
+        <v>2</v>
+      </c>
+      <c r="F60" s="29" t="s">
         <v>114</v>
-      </c>
-      <c r="E60" s="18">
-        <v>2</v>
-      </c>
-      <c r="F60" s="29" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2440,7 +2432,7 @@
         <v>6</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E61" s="18">
         <v>2</v>
@@ -2454,7 +2446,7 @@
         <v>6</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E62" s="18">
         <v>3</v>
@@ -2468,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E63" s="18">
         <v>2</v>
@@ -2485,7 +2477,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2500,29 +2492,27 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>173</v>
-      </c>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -2532,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -2549,13 +2539,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -2572,13 +2562,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -2595,13 +2585,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -2618,7 +2608,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2634,7 +2624,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2650,13 +2640,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -2673,13 +2663,13 @@
         <v>12</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -2696,13 +2686,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -2719,13 +2709,13 @@
         <v>16</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -2742,7 +2732,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2758,7 +2748,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2774,13 +2764,13 @@
         <v>19</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -2797,13 +2787,13 @@
         <v>20</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -2820,13 +2810,13 @@
         <v>21</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -2843,13 +2833,13 @@
         <v>22</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -2866,13 +2856,13 @@
         <v>24</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -2889,13 +2879,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -2912,13 +2902,13 @@
         <v>26</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -2935,13 +2925,13 @@
         <v>27</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -2958,13 +2948,13 @@
         <v>28</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F22" s="12">
         <v>1</v>
@@ -2981,13 +2971,13 @@
         <v>30</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F23" s="12">
         <v>5</v>
@@ -3004,13 +2994,13 @@
         <v>31</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F24" s="12">
         <v>5</v>
@@ -3027,13 +3017,13 @@
         <v>32</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F25" s="12">
         <v>7</v>
@@ -3050,13 +3040,13 @@
         <v>35</v>
       </c>
       <c r="C26" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F26" s="12">
         <v>1</v>
@@ -3073,7 +3063,7 @@
         <v>36</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -3087,7 +3077,7 @@
         <v>37</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -3101,13 +3091,13 @@
         <v>38</v>
       </c>
       <c r="C29" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F29" s="12">
         <v>1</v>
@@ -3124,13 +3114,13 @@
         <v>39</v>
       </c>
       <c r="C30" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F30" s="12">
         <v>1</v>
@@ -3147,13 +3137,13 @@
         <v>40</v>
       </c>
       <c r="C31" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F31" s="12">
         <v>5</v>
@@ -3170,13 +3160,13 @@
         <v>41</v>
       </c>
       <c r="C32" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F32" s="12">
         <v>1</v>
@@ -3193,13 +3183,13 @@
         <v>42</v>
       </c>
       <c r="C33" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F33" s="12">
         <v>1</v>
@@ -3216,7 +3206,7 @@
         <v>43</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -3230,13 +3220,13 @@
         <v>44</v>
       </c>
       <c r="C35" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F35" s="12">
         <v>1</v>
@@ -3253,13 +3243,13 @@
         <v>45</v>
       </c>
       <c r="C36" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F36" s="12">
         <v>1</v>
@@ -3276,13 +3266,13 @@
         <v>46</v>
       </c>
       <c r="C37" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F37" s="12">
         <v>1</v>
@@ -3299,13 +3289,13 @@
         <v>47</v>
       </c>
       <c r="C38" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F38" s="12">
         <v>1</v>
@@ -3322,13 +3312,13 @@
         <v>48</v>
       </c>
       <c r="C39" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F39" s="12">
         <v>1</v>
@@ -3345,13 +3335,13 @@
         <v>49</v>
       </c>
       <c r="C40" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F40" s="12">
         <v>1</v>
@@ -3368,13 +3358,13 @@
         <v>50</v>
       </c>
       <c r="C41" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F41" s="12">
         <v>1</v>
@@ -3391,13 +3381,13 @@
         <v>51</v>
       </c>
       <c r="C42" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F42" s="12">
         <v>1</v>
@@ -3414,7 +3404,7 @@
         <v>52</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -3428,13 +3418,13 @@
         <v>53</v>
       </c>
       <c r="C44" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F44" s="12">
         <v>1</v>
@@ -3451,13 +3441,13 @@
         <v>54</v>
       </c>
       <c r="C45" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F45" s="12">
         <v>1</v>
@@ -3474,13 +3464,13 @@
         <v>55</v>
       </c>
       <c r="C46" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="F46" s="12">
         <v>1</v>
@@ -3498,8 +3488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3514,20 +3504,18 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>173</v>
-      </c>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -3537,10 +3525,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -3552,10 +3540,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -3567,10 +3555,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -3582,10 +3570,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -3597,10 +3585,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -3612,10 +3600,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -3627,10 +3615,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -3642,10 +3630,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -3657,10 +3645,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -3672,10 +3660,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -3687,10 +3675,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -3702,10 +3690,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -3717,10 +3705,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -3732,10 +3720,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -3747,10 +3735,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -3762,10 +3750,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -3777,10 +3765,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -3792,10 +3780,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -3807,10 +3795,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -3822,10 +3810,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -3837,10 +3825,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -3852,10 +3840,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -3867,10 +3855,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="E24" s="1"/>
     </row>
@@ -3882,10 +3870,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>124</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3896,10 +3884,10 @@
         <v>4</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3910,10 +3898,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3924,10 +3912,10 @@
         <v>4</v>
       </c>
       <c r="C28" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="30" t="s">
         <v>136</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3938,10 +3926,10 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3952,10 +3940,10 @@
         <v>4</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3966,10 +3954,10 @@
         <v>4</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3980,10 +3968,10 @@
         <v>5</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3994,10 +3982,10 @@
         <v>5</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4008,10 +3996,10 @@
         <v>5</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4022,10 +4010,10 @@
         <v>5</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4036,10 +4024,10 @@
         <v>5</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4050,10 +4038,10 @@
         <v>6</v>
       </c>
       <c r="C37" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4064,10 +4052,10 @@
         <v>6</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4078,10 +4066,10 @@
         <v>6</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4092,10 +4080,10 @@
         <v>6</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4106,10 +4094,10 @@
         <v>6</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>